<commit_message>
Update salary calculator and documentation for tax regulations; adjust JP calculation limits
</commit_message>
<xml_diff>
--- a/src/ter.xlsx
+++ b/src/ter.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -52,7 +52,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
@@ -285,11 +285,11 @@
   </sheetPr>
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A99" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E107" activeCellId="0" sqref="E107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="13.68"/>

</xml_diff>